<commit_message>
correción ortografia, manejo de vacios y respuestas, en mettodo secante, regla falsa, lagrange, newtonint
</commit_message>
<xml_diff>
--- a/app/tables/tabla_newton.xlsx
+++ b/app/tables/tabla_newton.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-65.0</t>
+          <t>-74.1625989480318</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.000005</t>
+          <t>1.0000001</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.21424360312087</t>
+          <t>124.411454631511</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-26.6302712393383</t>
+          <t>-51.0785344246869</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.354864476416074</t>
+          <t>0.983924309815975</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.16674765448471</t>
+          <t>506.898276023503</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-13.678949962338</t>
+          <t>-12.4258528532728</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.897791347263332</t>
+          <t>0.754563271338208</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-1.77257584283229</t>
+          <t>655.511596189056</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-6.94363979939362</t>
+          <t>-0.539400249375262</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.65822157015321</t>
+          <t>0.226713487647732</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-3.66772137943643</t>
+          <t>662.540094232166</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3.44598839162184</t>
+          <t>-0.0009593573798554</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.516709242754788</t>
+          <t>0.0106084116331931</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-3.19849806177507</t>
+          <t>662.552639378594</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.218523634218298</t>
+          <t>-3.0275373319455e-09</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.14670114178558</t>
+          <t>1.89345656220124e-05</t>
         </is>
       </c>
     </row>
@@ -595,61 +595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-3.16442532963776</t>
+          <t>662.552639418184</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.0011475026314019</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.0107674312356769</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>-3.16424450940417</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>3.23050833219568e-08</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5.71448360112314e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>-3.16424450431334</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>-1.00093544563862e-15</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.6088614078435902e-09</t>
+          <t>5.97540305870696e-11</t>
         </is>
       </c>
     </row>

</xml_diff>